<commit_message>
Added Elements to elements data
</commit_message>
<xml_diff>
--- a/src/main/other/ElementsData.xlsx
+++ b/src/main/other/ElementsData.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\MEOCloud\ISEL\Git\Bootstrap\first\www\src\main\other\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="100">
   <si>
     <t>Lula</t>
   </si>
@@ -315,13 +310,22 @@
   </si>
   <si>
     <t>anossasurpresa.eu</t>
+  </si>
+  <si>
+    <t>Vitinho</t>
+  </si>
+  <si>
+    <t>Ru</t>
+  </si>
+  <si>
+    <t>Belinha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,12 +334,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -350,8 +360,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +423,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,7 +458,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -624,29 +635,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -660,8 +671,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -685,8 +696,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B3">
@@ -699,7 +710,7 @@
         <v>17</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E49" si="0">"_repo.add(new Element("""&amp;C3&amp;""", """&amp;A3&amp;""", "&amp;IF(B3=1,"true","false")&amp;"));"</f>
+        <f t="shared" ref="E3:E51" si="0">"_repo.add(new Element("""&amp;C3&amp;""", """&amp;A3&amp;""", "&amp;IF(B3=1,"true","false")&amp;"));"</f>
         <v>_repo.add(new Element("zgrfwk92", "&amp;Ecirc;lsio", true));</v>
       </c>
       <c r="F3" t="str">
@@ -710,8 +721,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B4">
@@ -728,15 +739,15 @@
         <v>_repo.add(new Element("wgbwmrhy", "Cl&amp;aacute;udio", true));</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F3:F49" si="1">"Olá! Este ano temos um presente especial, num formato diferente… Acede a "&amp;G4&amp;" insere o código "&amp;C4&amp;" e descobre a nossa surpresa de Natal! Inês e Ricardo"</f>
+        <f t="shared" ref="F4:F50" si="1">"Olá! Este ano temos um presente especial, num formato diferente… Acede a "&amp;G4&amp;" insere o código "&amp;C4&amp;" e descobre a nossa surpresa de Natal! Inês e Ricardo"</f>
         <v>Olá! Este ano temos um presente especial, num formato diferente… Acede a anossasurpresa.eu insere o código wgbwmrhy e descobre a nossa surpresa de Natal! Inês e Ricardo</v>
       </c>
       <c r="G4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B5">
@@ -760,8 +771,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B6">
@@ -785,8 +796,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B7">
@@ -810,8 +821,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B8">
@@ -835,8 +846,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B9">
@@ -860,8 +871,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B10">
@@ -885,8 +896,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B11">
@@ -910,8 +921,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7">
+      <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B12">
@@ -935,8 +946,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B13">
@@ -960,8 +971,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:7">
+      <c r="A14" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B14">
@@ -985,8 +996,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B15">
@@ -1010,8 +1021,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:7">
+      <c r="A16" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B16">
@@ -1035,8 +1046,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:7">
+      <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B17">
@@ -1060,8 +1071,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:7">
+      <c r="A18" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B18">
@@ -1085,8 +1096,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:7">
+      <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B19">
@@ -1110,8 +1121,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:7">
+      <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B20">
@@ -1135,8 +1146,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:7">
+      <c r="A21" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B21">
@@ -1160,8 +1171,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:7">
+      <c r="A22" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B22">
@@ -1185,8 +1196,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B23">
@@ -1210,8 +1221,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:7">
+      <c r="A24" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B24">
@@ -1235,8 +1246,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:7">
+      <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B25">
@@ -1260,8 +1271,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:7">
+      <c r="A26" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B26">
@@ -1285,8 +1296,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="27" spans="1:7">
+      <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B27">
@@ -1310,8 +1321,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="28" spans="1:7">
+      <c r="A28" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B28">
@@ -1335,8 +1346,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="29" spans="1:7">
+      <c r="A29" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B29">
@@ -1360,8 +1371,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="30" spans="1:7">
+      <c r="A30" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B30">
@@ -1385,8 +1396,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="31" spans="1:7">
+      <c r="A31" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B31">
@@ -1410,8 +1421,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="32" spans="1:7">
+      <c r="A32" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B32">
@@ -1435,8 +1446,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="33" spans="1:7">
+      <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B33">
@@ -1460,8 +1471,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="34" spans="1:7">
+      <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B34">
@@ -1485,8 +1496,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="35" spans="1:7">
+      <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B35">
@@ -1510,8 +1521,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="36" spans="1:7">
+      <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B36">
@@ -1535,8 +1546,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:7">
+      <c r="A37" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B37">
@@ -1560,8 +1571,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="38" spans="1:7">
+      <c r="A38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B38">
@@ -1585,8 +1596,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="39" spans="1:7">
+      <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B39">
@@ -1610,8 +1621,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:7">
+      <c r="A40" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B40">
@@ -1635,8 +1646,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="41" spans="1:7">
+      <c r="A41" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B41">
@@ -1660,8 +1671,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="42" spans="1:7">
+      <c r="A42" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B42">
@@ -1685,8 +1696,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="43" spans="1:7">
+      <c r="A43" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B43">
@@ -1710,8 +1721,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="44" spans="1:7">
+      <c r="A44" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B44">
@@ -1735,8 +1746,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="45" spans="1:7">
+      <c r="A45" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B45">
@@ -1760,8 +1771,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="46" spans="1:7">
+      <c r="A46" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B46">
@@ -1785,8 +1796,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="47" spans="1:7">
+      <c r="A47" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B47">
@@ -1810,8 +1821,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="48" spans="1:7">
+      <c r="A48" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B48">
@@ -1835,8 +1846,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="49" spans="1:7">
+      <c r="A49" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B49">
@@ -1857,6 +1868,81 @@
         <v>Olá! Este ano temos um presente especial, num formato diferente… Acede a anossasurpresa.eu insere o código eji85owt e descobre a nossa surpresa de Natal! Inês e Ricardo</v>
       </c>
       <c r="G49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="0"/>
+        <v>_repo.add(new Element("7r4tt5fe", "Ru", false));</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="1"/>
+        <v>Olá! Este ano temos um presente especial, num formato diferente… Acede a anossasurpresa.eu insere o código 7r4tt5fe e descobre a nossa surpresa de Natal! Inês e Ricardo</v>
+      </c>
+      <c r="G50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>97</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" ref="E51:E52" si="2">"_repo.add(new Element("""&amp;C51&amp;""", """&amp;A51&amp;""", "&amp;IF(B51=1,"true","false")&amp;"));"</f>
+        <v>_repo.add(new Element("kxujyo72", "Vitinho", true));</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" ref="F51" si="3">"Olá! Este ano temos um presente especial, num formato diferente… Acede a "&amp;G51&amp;" insere o código "&amp;C51&amp;" e descobre a nossa surpresa de Natal! Inês e Ricardo"</f>
+        <v>Olá! Este ano temos um presente especial, num formato diferente… Acede a anossasurpresa.eu insere o código kxujyo72 e descobre a nossa surpresa de Natal! Inês e Ricardo</v>
+      </c>
+      <c r="G51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>62</v>
+      </c>
+      <c r="D52" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="2"/>
+        <v>_repo.add(new Element("5jwzbhwk", "Belinha", false));</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" ref="F52" si="4">"Olá! Este ano temos um presente especial, num formato diferente… Acede a "&amp;G52&amp;" insere o código "&amp;C52&amp;" e descobre a nossa surpresa de Natal! Inês e Ricardo"</f>
+        <v>Olá! Este ano temos um presente especial, num formato diferente… Acede a anossasurpresa.eu insere o código 5jwzbhwk e descobre a nossa surpresa de Natal! Inês e Ricardo</v>
+      </c>
+      <c r="G52" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>